<commit_message>
sn: update Sénégal forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Senegal/TAS3/sn_lf_tas3_20305_2_partcipants.xlsx
+++ b/LF/TAS/Senegal/TAS3/sn_lf_tas3_20305_2_partcipants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Senegal\TAS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57FF385-6AE8-48A7-8916-4CDEAF7EF83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3309FB9-E595-4B14-94A0-EC5D324A9305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -348,10 +348,10 @@
     <t>French</t>
   </si>
   <si>
-    <t>sn_lf_tas3_20305_2_partcipants</t>
-  </si>
-  <si>
-    <t>(2023 Mai) 2. TAS1 FL - Formulaire Participants V2</t>
+    <t>(2023 Mai) 2. TAS(1-3) FL - Formulaire Participants V2.1</t>
+  </si>
+  <si>
+    <t>sn_lf_tas3_20305_2_partcipants_v2_1</t>
   </si>
 </sst>
 </file>
@@ -829,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1509,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1537,10 +1537,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>109</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>108</v>
       </c>
       <c r="C2" s="30">
         <v>20210419</v>

</xml_diff>